<commit_message>
esto es otra actualizacion
</commit_message>
<xml_diff>
--- a/test-export-fixed.xlsx
+++ b/test-export-fixed.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="119">
   <si>
     <t>ALCALDÍA MUNICIPAL DE GUADALAJARA DE BUGA</t>
   </si>
@@ -46,13 +46,13 @@
     <t>Página 1 de 1</t>
   </si>
   <si>
-    <t>NUMERO DE CONTRATO: CONTRATO-TEST-001</t>
-  </si>
-  <si>
-    <t>VALOR: $50.000.000</t>
-  </si>
-  <si>
-    <t>CONTRATISTA: CONTRATISTA DE PRUEBA SAS</t>
+    <t>NUMERO DE CONTRATO: 001-005</t>
+  </si>
+  <si>
+    <t>VALOR: $10.000.000</t>
+  </si>
+  <si>
+    <t>CONTRATISTA: Cristofer</t>
   </si>
   <si>
     <t>ETAPA PRECONTRACTUAL</t>
@@ -224,21 +224,6 @@
   </si>
   <si>
     <t>ACTA DE LIQUIDACIÓN</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Observación de prueba 1</t>
-  </si>
-  <si>
-    <t>Observación de prueba 2</t>
-  </si>
-  <si>
-    <t>Observación de prueba 3</t>
   </si>
   <si>
     <t>CODIGO: ASE.BYS.SP-01.PR-01-F5</t>
@@ -1561,7 +1546,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I304"/>
+  <dimension ref="A1:E64"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100" view="pageBreakPreview">
       <selection activeCell="D46" sqref="D46"/>
@@ -2264,63 +2249,6 @@
       <c r="C64" s="39"/>
       <c r="D64" s="39"/>
       <c r="E64" s="40"/>
-    </row>
-    <row r="266" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A266" s="1"/>
-      <c r="B266" s="2"/>
-      <c r="C266" s="2"/>
-      <c r="D266" s="2"/>
-      <c r="E266" s="2"/>
-      <c r="F266" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="G266" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="H266" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="I266" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="287" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A287" s="1"/>
-      <c r="B287" s="2"/>
-      <c r="C287" s="2"/>
-      <c r="D287" s="2"/>
-      <c r="E287" s="2"/>
-      <c r="F287" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G287" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="H287" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="I287" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="304" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A304" s="1"/>
-      <c r="B304" s="2"/>
-      <c r="C304" s="2"/>
-      <c r="D304" s="2"/>
-      <c r="E304" s="2"/>
-      <c r="F304" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G304" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="H304" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="I304" s="2" t="s">
-        <v>71</v>
-      </c>
     </row>
   </sheetData>
   <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" algorithmName="SHA-512" hashValue="QFexg9U1bNGeHLFpySnlCGlUFOR0JqkCAe3RL5kMQBsrpgythaPOZFn2Er7U6DWNFyllKQ33X05OfZ+eYz8HPw==" saltValue="IU/4vAu3u0FE+twI4jdynw==" spinCount="100000" objects="1" scenarios="1"/>
@@ -2347,7 +2275,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I304"/>
+  <dimension ref="A1:F64"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100" view="pageBreakPreview">
       <selection activeCell="C56" sqref="C56"/>
@@ -2372,7 +2300,7 @@
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="5" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" ht="15" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -2398,7 +2326,7 @@
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="4" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -2733,7 +2661,7 @@
         <v>24</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C35" s="21"/>
       <c r="D35" s="21"/>
@@ -3057,63 +2985,6 @@
       <c r="C64" s="39"/>
       <c r="D64" s="39"/>
       <c r="E64" s="40"/>
-    </row>
-    <row r="266" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A266" s="41"/>
-      <c r="B266" s="42"/>
-      <c r="C266" s="42"/>
-      <c r="D266" s="42"/>
-      <c r="E266" s="42"/>
-      <c r="F266" s="42" t="s">
-        <v>67</v>
-      </c>
-      <c r="G266" s="42" t="s">
-        <v>68</v>
-      </c>
-      <c r="H266" s="42" t="s">
-        <v>68</v>
-      </c>
-      <c r="I266" s="42" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="287" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A287" s="41"/>
-      <c r="B287" s="42"/>
-      <c r="C287" s="42"/>
-      <c r="D287" s="42"/>
-      <c r="E287" s="42"/>
-      <c r="F287" s="42" t="s">
-        <v>68</v>
-      </c>
-      <c r="G287" s="42" t="s">
-        <v>67</v>
-      </c>
-      <c r="H287" s="42" t="s">
-        <v>68</v>
-      </c>
-      <c r="I287" s="42" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="304" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A304" s="41"/>
-      <c r="B304" s="42"/>
-      <c r="C304" s="42"/>
-      <c r="D304" s="42"/>
-      <c r="E304" s="42"/>
-      <c r="F304" s="42" t="s">
-        <v>68</v>
-      </c>
-      <c r="G304" s="42" t="s">
-        <v>68</v>
-      </c>
-      <c r="H304" s="42" t="s">
-        <v>67</v>
-      </c>
-      <c r="I304" s="42" t="s">
-        <v>71</v>
-      </c>
     </row>
   </sheetData>
   <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" sort="0" autoFilter="0" pivotTables="0" algorithmName="SHA-512" hashValue="dulMRaEAKguAY96e7cQcLXx6UUDub9HHpv8gC3uG7n8N5TfGMAJ4BtTZHNk3343JKeMl6ND9x7r46GuHc08m/w==" saltValue="upU4zaP4YyKNqtF3eIDw6w==" spinCount="100000"/>
@@ -3140,7 +3011,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I304"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100" view="pageBreakPreview">
       <selection activeCell="B38" sqref="B38"/>
@@ -3164,7 +3035,7 @@
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="5" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" ht="15" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -3190,7 +3061,7 @@
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -3281,7 +3152,7 @@
         <v>2</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C13" s="21"/>
       <c r="D13" s="21"/>
@@ -3292,7 +3163,7 @@
         <v>3</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C14" s="21"/>
       <c r="D14" s="21"/>
@@ -3303,7 +3174,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C15" s="21"/>
       <c r="D15" s="21"/>
@@ -3314,7 +3185,7 @@
         <v>5</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C16" s="21"/>
       <c r="D16" s="21"/>
@@ -3325,7 +3196,7 @@
         <v>6</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C17" s="21"/>
       <c r="D17" s="21"/>
@@ -3347,7 +3218,7 @@
         <v>8</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C19" s="21"/>
       <c r="D19" s="21"/>
@@ -3358,7 +3229,7 @@
         <v>9</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C20" s="21"/>
       <c r="D20" s="21"/>
@@ -3391,7 +3262,7 @@
         <v>12</v>
       </c>
       <c r="B23" s="58" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C23" s="59"/>
       <c r="D23" s="59"/>
@@ -3411,7 +3282,7 @@
         <v>13</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C25" s="21"/>
       <c r="D25" s="21"/>
@@ -3466,7 +3337,7 @@
         <v>18</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C30" s="21"/>
       <c r="D30" s="21"/>
@@ -3477,7 +3348,7 @@
         <v>19</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C31" s="21"/>
       <c r="D31" s="21"/>
@@ -3499,7 +3370,7 @@
         <v>21</v>
       </c>
       <c r="B33" s="61" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C33" s="62"/>
       <c r="D33" s="62"/>
@@ -3601,63 +3472,6 @@
       <c r="C42" s="39"/>
       <c r="D42" s="39"/>
       <c r="E42" s="40"/>
-    </row>
-    <row r="266" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A266" s="1"/>
-      <c r="B266" s="2"/>
-      <c r="C266" s="2"/>
-      <c r="D266" s="2"/>
-      <c r="E266" s="2"/>
-      <c r="F266" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="G266" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="H266" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="I266" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="287" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A287" s="1"/>
-      <c r="B287" s="2"/>
-      <c r="C287" s="2"/>
-      <c r="D287" s="2"/>
-      <c r="E287" s="2"/>
-      <c r="F287" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G287" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="H287" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="I287" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="304" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A304" s="1"/>
-      <c r="B304" s="2"/>
-      <c r="C304" s="2"/>
-      <c r="D304" s="2"/>
-      <c r="E304" s="2"/>
-      <c r="F304" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G304" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="H304" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="I304" s="2" t="s">
-        <v>71</v>
-      </c>
     </row>
   </sheetData>
   <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" sort="0" autoFilter="0" pivotTables="0" algorithmName="SHA-512" hashValue="0B0rBHmnKiMGL+/+x2HlJVNQXnOuP1FeXY+Ljaa1A3tKGoDg6RLVZhkfENyjlCX4sMOIZ2hOllOaBH1io+wktw==" saltValue="wUqpPqmn1fLVIJgRwtrQgQ==" spinCount="100000"/>
@@ -3684,7 +3498,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I304"/>
+  <dimension ref="A1:E65"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100" view="pageBreakPreview">
       <selection activeCell="C13" sqref="C13"/>
@@ -3708,7 +3522,7 @@
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="5" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" ht="15" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -3734,7 +3548,7 @@
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="4" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -3814,7 +3628,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C12" s="21"/>
       <c r="D12" s="21"/>
@@ -3825,7 +3639,7 @@
         <v>2</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C13" s="21"/>
       <c r="D13" s="21"/>
@@ -3836,7 +3650,7 @@
         <v>3</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C14" s="21"/>
       <c r="D14" s="21"/>
@@ -3847,7 +3661,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C15" s="21"/>
       <c r="D15" s="21"/>
@@ -3869,7 +3683,7 @@
         <v>6</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C17" s="21"/>
       <c r="D17" s="21"/>
@@ -3880,7 +3694,7 @@
         <v>7</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C18" s="21"/>
       <c r="D18" s="21"/>
@@ -3891,7 +3705,7 @@
         <v>8</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C19" s="21"/>
       <c r="D19" s="21"/>
@@ -3979,7 +3793,7 @@
         <v>16</v>
       </c>
       <c r="B27" s="20" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C27" s="21"/>
       <c r="D27" s="21"/>
@@ -3990,7 +3804,7 @@
         <v>17</v>
       </c>
       <c r="B28" s="20" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C28" s="21"/>
       <c r="D28" s="21"/>
@@ -4001,7 +3815,7 @@
         <v>18</v>
       </c>
       <c r="B29" s="20" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C29" s="21"/>
       <c r="D29" s="21"/>
@@ -4012,7 +3826,7 @@
         <v>19</v>
       </c>
       <c r="B30" s="20" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C30" s="21"/>
       <c r="D30" s="21"/>
@@ -4023,7 +3837,7 @@
         <v>20</v>
       </c>
       <c r="B31" s="20" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C31" s="21"/>
       <c r="D31" s="21"/>
@@ -4034,7 +3848,7 @@
         <v>21</v>
       </c>
       <c r="B32" s="20" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C32" s="21"/>
       <c r="D32" s="21"/>
@@ -4045,7 +3859,7 @@
         <v>22</v>
       </c>
       <c r="B33" s="58" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C33" s="59"/>
       <c r="D33" s="59"/>
@@ -4087,7 +3901,7 @@
         <v>25</v>
       </c>
       <c r="B37" s="20" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C37" s="72"/>
       <c r="D37" s="72"/>
@@ -4098,7 +3912,7 @@
         <v>26</v>
       </c>
       <c r="B38" s="20" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C38" s="72"/>
       <c r="D38" s="72"/>
@@ -4120,7 +3934,7 @@
         <v>28</v>
       </c>
       <c r="B40" s="20" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C40" s="35"/>
       <c r="D40" s="35"/>
@@ -4131,7 +3945,7 @@
         <v>29</v>
       </c>
       <c r="B41" s="58" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C41" s="35"/>
       <c r="D41" s="35"/>
@@ -4142,7 +3956,7 @@
         <v>30</v>
       </c>
       <c r="B42" s="58" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C42" s="35"/>
       <c r="D42" s="35"/>
@@ -4164,7 +3978,7 @@
         <v>32</v>
       </c>
       <c r="B44" s="38" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C44" s="39"/>
       <c r="D44" s="39"/>
@@ -4206,7 +4020,7 @@
         <v>35</v>
       </c>
       <c r="B48" s="20" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C48" s="35"/>
       <c r="D48" s="35"/>
@@ -4247,7 +4061,7 @@
     </row>
     <row r="52" ht="17.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="31" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B52" s="32"/>
       <c r="C52" s="32"/>
@@ -4259,7 +4073,7 @@
         <v>39</v>
       </c>
       <c r="B53" s="74" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C53" s="35"/>
       <c r="D53" s="35"/>
@@ -4270,7 +4084,7 @@
         <v>40</v>
       </c>
       <c r="B54" s="74" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C54" s="35"/>
       <c r="D54" s="35"/>
@@ -4281,7 +4095,7 @@
         <v>41</v>
       </c>
       <c r="B55" s="74" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C55" s="35"/>
       <c r="D55" s="35"/>
@@ -4292,7 +4106,7 @@
         <v>42</v>
       </c>
       <c r="B56" s="74" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C56" s="35"/>
       <c r="D56" s="35"/>
@@ -4314,7 +4128,7 @@
         <v>44</v>
       </c>
       <c r="B58" s="74" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C58" s="35"/>
       <c r="D58" s="35"/>
@@ -4325,7 +4139,7 @@
         <v>45</v>
       </c>
       <c r="B59" s="74" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C59" s="35"/>
       <c r="D59" s="35"/>
@@ -4336,7 +4150,7 @@
         <v>46</v>
       </c>
       <c r="B60" s="74" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C60" s="35"/>
       <c r="D60" s="35"/>
@@ -4347,7 +4161,7 @@
         <v>47</v>
       </c>
       <c r="B61" s="74" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C61" s="35"/>
       <c r="D61" s="35"/>
@@ -4358,7 +4172,7 @@
         <v>48</v>
       </c>
       <c r="B62" s="74" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C62" s="35"/>
       <c r="D62" s="35"/>
@@ -4369,7 +4183,7 @@
         <v>49</v>
       </c>
       <c r="B63" s="74" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C63" s="35"/>
       <c r="D63" s="35"/>
@@ -4380,7 +4194,7 @@
         <v>50</v>
       </c>
       <c r="B64" s="74" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C64" s="35"/>
       <c r="D64" s="35"/>
@@ -4391,68 +4205,11 @@
         <v>51</v>
       </c>
       <c r="B65" s="74" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C65" s="35"/>
       <c r="D65" s="35"/>
       <c r="E65" s="36"/>
-    </row>
-    <row r="266" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A266" s="1"/>
-      <c r="B266" s="2"/>
-      <c r="C266" s="2"/>
-      <c r="D266" s="2"/>
-      <c r="E266" s="2"/>
-      <c r="F266" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="G266" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="H266" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="I266" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="287" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A287" s="1"/>
-      <c r="B287" s="2"/>
-      <c r="C287" s="2"/>
-      <c r="D287" s="2"/>
-      <c r="E287" s="2"/>
-      <c r="F287" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G287" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="H287" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="I287" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="304" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A304" s="1"/>
-      <c r="B304" s="2"/>
-      <c r="C304" s="2"/>
-      <c r="D304" s="2"/>
-      <c r="E304" s="2"/>
-      <c r="F304" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G304" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="H304" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="I304" s="2" t="s">
-        <v>71</v>
-      </c>
     </row>
   </sheetData>
   <sheetProtection sheet="1" algorithmName="SHA-512" hashValue="hDHYJRONK1sQ5ZhyLwnqb7nzj45AgCbYFjZAGVZUJLWYtxtaMaFurL5NL771Zd00bD6TenGtAL7noTbxs//DBw==" saltValue="2vvest3Xsqfk+qM1+sWmWA==" spinCount="100000" objects="1" scenarios="1"/>

</xml_diff>